<commit_message>
Added a negative test as well
</commit_message>
<xml_diff>
--- a/src/data/excel.xlsx
+++ b/src/data/excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayakaushik\Main_Assignment_Selenium\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0100D352-5FF5-4DF0-AF7A-68F5E191D4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163EB61F-977C-4F82-9DF3-01A2B8BC3E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Mayank</t>
   </si>
   <si>
     <t>Kaushik</t>
-  </si>
-  <si>
-    <t>asdasda</t>
   </si>
 </sst>
 </file>
@@ -366,8 +363,8 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="C1">
+        <v>201005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pom changes and read write from excel
</commit_message>
<xml_diff>
--- a/src/data/excel.xlsx
+++ b/src/data/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayakaushik\Main_Assignment_Selenium\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163EB61F-977C-4F82-9DF3-01A2B8BC3E59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8874E693-FBFE-4ACA-AC65-5AE9D8715B6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mayank</t>
   </si>
   <si>
     <t>Kaushik</t>
+  </si>
+  <si>
+    <t>E12312</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>fname</t>
   </si>
 </sst>
 </file>
@@ -348,23 +360,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>201005</v>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>